<commit_message>
exams examples from course website, GenFun in Rosen
</commit_message>
<xml_diff>
--- a/Exams/משקל נושאים.xlsx
+++ b/Exams/משקל נושאים.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared-dir\discrete_math\Exams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16E82D7-57D7-4FF1-A7CA-CE69D0222333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA99D525-FDA1-44A3-B688-637A1BBA3A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{63D0AE89-63A2-429A-B285-D79EF76DC49F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63D0AE89-63A2-429A-B285-D79EF76DC49F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>לוגיקה</t>
   </si>
@@ -54,13 +54,16 @@
     <t>עוצמות</t>
   </si>
   <si>
-    <t>קומבינטוריקה כללי</t>
-  </si>
-  <si>
     <t>14+14+13 = 41</t>
   </si>
   <si>
     <t>27 + 9 = 36</t>
+  </si>
+  <si>
+    <t>2019b_moed_b</t>
+  </si>
+  <si>
+    <t>קומבינטוריקה מחרוזות ונסיגה</t>
   </si>
 </sst>
 </file>
@@ -421,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B04E3A7-31FA-45D8-83F8-CF5B370740C0}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.77734375" customWidth="1"/>
     <col min="7" max="7" width="25.109375" customWidth="1"/>
     <col min="8" max="8" width="16.109375" customWidth="1"/>
@@ -455,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -582,41 +585,20 @@
         <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2018.83</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>27</v>
-      </c>
-      <c r="G7">
-        <v>27</v>
-      </c>
-      <c r="H7">
-        <v>27</v>
+      <c r="A7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>2018.84</v>
+        <v>2018.83</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -642,13 +624,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>2018.94</v>
+        <v>2018.84</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -657,38 +639,64 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>27</v>
       </c>
       <c r="H9">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
+        <v>2018.94</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>2018.85</v>
       </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>27</v>
-      </c>
-      <c r="G10">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>27</v>
+      </c>
+      <c r="G11">
         <v>54</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
combined all example exams from site, comb.docx includes all gen fns
</commit_message>
<xml_diff>
--- a/Exams/משקל נושאים.xlsx
+++ b/Exams/משקל נושאים.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared-dir\discrete_math\Exams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA99D525-FDA1-44A3-B688-637A1BBA3A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18F9892-D5BE-4FBD-9424-EDD27AA56DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63D0AE89-63A2-429A-B285-D79EF76DC49F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{63D0AE89-63A2-429A-B285-D79EF76DC49F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,6 +595,12 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">

</xml_diff>